<commit_message>
Automatizar actualización diaria de precios desde Excel
</commit_message>
<xml_diff>
--- a/PreciosP.xlsx
+++ b/PreciosP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/928767bb5677b83e/ECE CONSULTORES/VM PRECIOS A FUTURO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\calculadora-energia\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{B3244113-4520-4554-8B4C-2768291C762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D1652EE-ACF6-4C24-84FE-16B23051B749}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D57247-67D6-4103-AEC4-12596A21FFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01D25416-3606-4CF3-ADEB-58FCB3C46A56}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
   <si>
     <t>FEE</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>FACTURA PROPUESTA CON ESTOS PRECIOS</t>
+  </si>
+  <si>
+    <t>PRECIOS REFERENCIA</t>
+  </si>
+  <si>
+    <t>APUNTAL.</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1145,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1444,15 +1446,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947718FF-DCB1-496A-BB9E-193C0BA22031}">
   <dimension ref="A1:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.54296875" customWidth="1"/>
     <col min="8" max="8" width="15.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" customWidth="1"/>
+    <col min="14" max="14" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1472,10 +1474,10 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="31" t="s">
         <v>38</v>

</xml_diff>